<commit_message>
add: Srjk (interface & mean calculation)
</commit_message>
<xml_diff>
--- a/template_nilai_IPA.xlsx
+++ b/template_nilai_IPA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7530"/>
+    <workbookView windowWidth="10245" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="XII IPA SEMUA MAPEL" sheetId="4" r:id="rId1"/>
@@ -1094,8 +1094,8 @@
   <sheetPr/>
   <dimension ref="A1:CA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="AN4" workbookViewId="0">
-      <selection activeCell="BY18" sqref="BY18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.95" customHeight="1"/>
@@ -1442,7 +1442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:79">
+    <row r="5" ht="12.75" spans="1:79">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="8"/>
@@ -1523,7 +1523,7 @@
       <c r="BZ5" s="17"/>
       <c r="CA5" s="18"/>
     </row>
-    <row r="6" spans="1:79">
+    <row r="6" ht="12.75" spans="1:79">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="8"/>
@@ -1604,7 +1604,7 @@
       <c r="BZ6" s="17"/>
       <c r="CA6" s="18"/>
     </row>
-    <row r="7" spans="1:79">
+    <row r="7" ht="12.75" spans="1:79">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="8"/>
@@ -1685,7 +1685,7 @@
       <c r="BZ7" s="17"/>
       <c r="CA7" s="18"/>
     </row>
-    <row r="8" spans="1:79">
+    <row r="8" ht="12.75" spans="1:79">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="8"/>
@@ -1766,7 +1766,7 @@
       <c r="BZ8" s="17"/>
       <c r="CA8" s="18"/>
     </row>
-    <row r="9" spans="1:79">
+    <row r="9" ht="12.75" spans="1:79">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="8"/>
@@ -1847,7 +1847,7 @@
       <c r="BZ9" s="17"/>
       <c r="CA9" s="18"/>
     </row>
-    <row r="10" spans="1:79">
+    <row r="10" ht="12.75" spans="1:79">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="8"/>
@@ -1928,7 +1928,7 @@
       <c r="BZ10" s="17"/>
       <c r="CA10" s="18"/>
     </row>
-    <row r="11" spans="1:79">
+    <row r="11" ht="12.75" spans="1:79">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="8"/>
@@ -2009,7 +2009,7 @@
       <c r="BZ11" s="17"/>
       <c r="CA11" s="18"/>
     </row>
-    <row r="12" spans="1:79">
+    <row r="12" ht="12.75" spans="1:79">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="8"/>
@@ -2090,7 +2090,7 @@
       <c r="BZ12" s="17"/>
       <c r="CA12" s="18"/>
     </row>
-    <row r="13" spans="1:79">
+    <row r="13" ht="12.75" spans="1:79">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="8"/>
@@ -2171,7 +2171,7 @@
       <c r="BZ13" s="17"/>
       <c r="CA13" s="18"/>
     </row>
-    <row r="14" spans="1:79">
+    <row r="14" ht="12.75" spans="1:79">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="8"/>
@@ -2252,7 +2252,7 @@
       <c r="BZ14" s="17"/>
       <c r="CA14" s="18"/>
     </row>
-    <row r="15" spans="1:79">
+    <row r="15" ht="12.75" spans="1:79">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="8"/>
@@ -2333,7 +2333,7 @@
       <c r="BZ15" s="17"/>
       <c r="CA15" s="18"/>
     </row>
-    <row r="16" spans="1:79">
+    <row r="16" ht="12.75" spans="1:79">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="8"/>
@@ -2414,7 +2414,7 @@
       <c r="BZ16" s="17"/>
       <c r="CA16" s="18"/>
     </row>
-    <row r="17" spans="1:79">
+    <row r="17" ht="12.75" spans="1:79">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
@@ -2495,7 +2495,7 @@
       <c r="BZ17" s="17"/>
       <c r="CA17" s="18"/>
     </row>
-    <row r="18" spans="1:79">
+    <row r="18" ht="12.75" spans="1:79">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="8"/>
@@ -2576,7 +2576,7 @@
       <c r="BZ18" s="17"/>
       <c r="CA18" s="18"/>
     </row>
-    <row r="19" spans="1:79">
+    <row r="19" ht="12.75" spans="1:79">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="8"/>
@@ -2657,7 +2657,7 @@
       <c r="BZ19" s="17"/>
       <c r="CA19" s="18"/>
     </row>
-    <row r="20" spans="1:79">
+    <row r="20" ht="12.75" spans="1:79">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="8"/>
@@ -2738,7 +2738,7 @@
       <c r="BZ20" s="17"/>
       <c r="CA20" s="18"/>
     </row>
-    <row r="21" spans="1:79">
+    <row r="21" ht="12.75" spans="1:79">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="8"/>
@@ -2819,7 +2819,7 @@
       <c r="BZ21" s="17"/>
       <c r="CA21" s="18"/>
     </row>
-    <row r="22" spans="1:79">
+    <row r="22" ht="12.75" spans="1:79">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="8"/>
@@ -2900,7 +2900,7 @@
       <c r="BZ22" s="17"/>
       <c r="CA22" s="18"/>
     </row>
-    <row r="23" spans="1:79">
+    <row r="23" ht="12.75" spans="1:79">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="8"/>
@@ -2981,7 +2981,7 @@
       <c r="BZ23" s="17"/>
       <c r="CA23" s="18"/>
     </row>
-    <row r="24" spans="1:79">
+    <row r="24" ht="12.75" spans="1:79">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="8"/>
@@ -3062,7 +3062,7 @@
       <c r="BZ24" s="17"/>
       <c r="CA24" s="18"/>
     </row>
-    <row r="25" spans="1:79">
+    <row r="25" ht="12.75" spans="1:79">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="8"/>
@@ -3143,7 +3143,7 @@
       <c r="BZ25" s="17"/>
       <c r="CA25" s="18"/>
     </row>
-    <row r="26" spans="1:79">
+    <row r="26" ht="12.75" spans="1:79">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="8"/>
@@ -3224,7 +3224,7 @@
       <c r="BZ26" s="17"/>
       <c r="CA26" s="18"/>
     </row>
-    <row r="27" spans="1:79">
+    <row r="27" ht="12.75" spans="1:79">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="8"/>
@@ -3305,7 +3305,7 @@
       <c r="BZ27" s="17"/>
       <c r="CA27" s="18"/>
     </row>
-    <row r="28" spans="1:79">
+    <row r="28" ht="12.75" spans="1:79">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="8"/>
@@ -3386,7 +3386,7 @@
       <c r="BZ28" s="17"/>
       <c r="CA28" s="18"/>
     </row>
-    <row r="29" spans="1:79">
+    <row r="29" ht="12.75" spans="1:79">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="8"/>
@@ -3467,7 +3467,7 @@
       <c r="BZ29" s="17"/>
       <c r="CA29" s="18"/>
     </row>
-    <row r="30" spans="1:79">
+    <row r="30" ht="12.75" spans="1:79">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="8"/>
@@ -3548,7 +3548,7 @@
       <c r="BZ30" s="17"/>
       <c r="CA30" s="18"/>
     </row>
-    <row r="31" spans="1:79">
+    <row r="31" ht="12.75" spans="1:79">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="8"/>
@@ -3629,7 +3629,7 @@
       <c r="BZ31" s="17"/>
       <c r="CA31" s="18"/>
     </row>
-    <row r="32" spans="1:79">
+    <row r="32" ht="12.75" spans="1:79">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="8"/>
@@ -3710,7 +3710,7 @@
       <c r="BZ32" s="17"/>
       <c r="CA32" s="18"/>
     </row>
-    <row r="33" spans="1:79">
+    <row r="33" ht="12.75" spans="1:79">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="8"/>
@@ -3791,7 +3791,7 @@
       <c r="BZ33" s="17"/>
       <c r="CA33" s="18"/>
     </row>
-    <row r="34" spans="1:79">
+    <row r="34" ht="12.75" spans="1:79">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="8"/>
@@ -3872,7 +3872,7 @@
       <c r="BZ34" s="17"/>
       <c r="CA34" s="18"/>
     </row>
-    <row r="35" spans="1:79">
+    <row r="35" ht="12.75" spans="1:79">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
       <c r="C35" s="8"/>
@@ -3953,7 +3953,7 @@
       <c r="BZ35" s="17"/>
       <c r="CA35" s="18"/>
     </row>
-    <row r="36" spans="1:79">
+    <row r="36" ht="12.75" spans="1:79">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
       <c r="C36" s="8"/>
@@ -4034,7 +4034,7 @@
       <c r="BZ36" s="17"/>
       <c r="CA36" s="18"/>
     </row>
-    <row r="37" spans="1:79">
+    <row r="37" ht="12.75" spans="1:79">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
       <c r="C37" s="8"/>

</xml_diff>